<commit_message>
made mistake in esp32 feather pin spacing; should be 800 mil, not 900 mil
</commit_message>
<xml_diff>
--- a/Keyboard_Bottom/Project Outputs for Keyboard_Bottom/BOM/Bill of Materials-Keyboard_Bottom.xlsx
+++ b/Keyboard_Bottom/Project Outputs for Keyboard_Bottom/BOM/Bill of Materials-Keyboard_Bottom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\college\osu_keyboard\Keyboard_Bottom\Project Outputs for Keyboard_Bottom\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3317263B-60C2-4CFB-90EC-F3CB79C5C7F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D400CA3-B2CA-435D-94B8-D3712DDD63AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{65D7688D-1A56-4B04-9BE5-1F4B11C6195E}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{EDE89946-E5B7-4613-A8DD-FB142B6D1B55}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-Keyboard_Bott" sheetId="1" r:id="rId1"/>
@@ -601,7 +601,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAEF8DC6-F2C7-4831-8072-152267160925}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1F496DA-59DF-416C-A592-6CB295498164}">
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>